<commit_message>
added class , inheritence and exception handling
</commit_message>
<xml_diff>
--- a/selected_data.xlsx
+++ b/selected_data.xlsx
@@ -446,22 +446,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>99004391.0</t>
+          <t>99004392.0</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>god of war</t>
+          <t>midnight children</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>gears of war 5</t>
+          <t>catcher in rye</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>forza horizon 5</t>
+          <t>animal farm</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added large excel file
</commit_message>
<xml_diff>
--- a/selected_data.xlsx
+++ b/selected_data.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -427,41 +427,111 @@
           <t>psno</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>one</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>two</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>three</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>99004392.0</t>
+          <t>99004400.0</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>midnight children</t>
+          <t>mordern family</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>catcher in rye</t>
+          <t>cyberpunk</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>animal farm</t>
+          <t>mirzapur</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>anupama</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>cyberpunk</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>ac origins</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>mordern family</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>cyberpunk 2077</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>ac valhalla</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>resident evil</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>cyberpunk</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>ac valhalla</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>writer's legacy</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>two</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>ac origins</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">resident evil5 </t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>euphoria</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>mare easttown</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>friends</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>two</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added exception and unit tests
</commit_message>
<xml_diff>
--- a/selected_data.xlsx
+++ b/selected_data.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U2"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -428,113 +428,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>99004405.0</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>alice in borderland</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>horizon forbidden</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>mare easttown</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">gta </t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>horizon forbidden</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>fortnite 2021</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>alice in borderland</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>horizon forbidden east</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>fortnite</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>fifa 21</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>horizon forbidden</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>fortnite</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>blacklist</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>young sheldon</t>
-        </is>
-      </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>fortnite 2021</t>
-        </is>
-      </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>fifa 15</t>
-        </is>
-      </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>horizon forbidden east</t>
-        </is>
-      </c>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t>mordern family</t>
-        </is>
-      </c>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t>horizon forbidden east</t>
-        </is>
-      </c>
-      <c r="U2" t="inlineStr">
-        <is>
-          <t>fortnite</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>